<commit_message>
added scale for 1mL syringe
</commit_message>
<xml_diff>
--- a/data/commerical-Vs-printed-comparison/data-taking-raw/reading_vs_weight160225.xlsx
+++ b/data/commerical-Vs-printed-comparison/data-taking-raw/reading_vs_weight160225.xlsx
@@ -1,28 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26722"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fahad\Documents\Git Bash\micropipette\micropipette\data\commerical-Vs-printed-comparison\data-taking-raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="0" windowWidth="20360" windowHeight="13800"/>
+    <workbookView xWindow="2865" yWindow="0" windowWidth="20355" windowHeight="13800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Shee1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t xml:space="preserve">Reading </t>
   </si>
@@ -46,6 +52,18 @@
   </si>
   <si>
     <t>3ml</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Setting</t>
+  </si>
+  <si>
+    <t>Distance Amount</t>
+  </si>
+  <si>
+    <t>Distance Travel</t>
   </si>
 </sst>
 </file>
@@ -138,9 +156,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -222,7 +241,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -252,11 +270,10 @@
           </c:spPr>
           <c:trendline>
             <c:trendlineType val="linear"/>
-            <c:intercept val="0.0"/>
+            <c:intercept val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -267,19 +284,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>205.0</c:v>
+                  <c:v>205</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>310.0</c:v>
+                  <c:v>310</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -291,19 +308,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9.73686</c:v>
+                  <c:v>9.7368600000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.54064000000004</c:v>
+                  <c:v>19.540640000000035</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49.48734</c:v>
+                  <c:v>49.487339999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>200.76</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>300.8054000000004</c:v>
+                  <c:v>300.80540000000036</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -318,11 +335,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2103421320"/>
-        <c:axId val="2103424136"/>
+        <c:axId val="-378886896"/>
+        <c:axId val="-378885808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2103421320"/>
+        <c:axId val="-378886896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -332,12 +349,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2103424136"/>
+        <c:crossAx val="-378885808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2103424136"/>
+        <c:axId val="-378885808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -348,14 +365,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2103421320"/>
+        <c:crossAx val="-378886896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -364,7 +380,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -400,7 +416,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -430,11 +445,10 @@
           </c:spPr>
           <c:trendline>
             <c:trendlineType val="linear"/>
-            <c:intercept val="0.0"/>
+            <c:intercept val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -445,19 +459,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>205.0</c:v>
+                  <c:v>205</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>310.0</c:v>
+                  <c:v>310</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>525.0</c:v>
+                  <c:v>525</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1030.0</c:v>
+                  <c:v>1030</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -469,19 +483,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>99.94502000000004</c:v>
+                  <c:v>99.945020000000042</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>201.7638</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.8723199999997</c:v>
+                  <c:v>300.87231999999966</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>502.10076</c:v>
+                  <c:v>502.10075999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1004.971100000003</c:v>
+                  <c:v>1004.9711000000034</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -496,11 +510,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2102620616"/>
-        <c:axId val="2102617800"/>
+        <c:axId val="-378884720"/>
+        <c:axId val="-378894512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2102620616"/>
+        <c:axId val="-378884720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -510,12 +524,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102617800"/>
+        <c:crossAx val="-378894512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2102617800"/>
+        <c:axId val="-378894512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -526,14 +540,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102620616"/>
+        <c:crossAx val="-378884720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -542,7 +555,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -868,7 +881,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -878,13 +891,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -892,7 +905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -906,7 +919,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>205</v>
       </c>
@@ -920,7 +933,7 @@
         <v>1000.4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>205</v>
       </c>
@@ -934,7 +947,7 @@
         <v>1001.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>205</v>
       </c>
@@ -948,7 +961,7 @@
         <v>1001.6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1">
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>AVERAGE(A3:A5)</f>
         <v>205</v>
@@ -966,7 +979,7 @@
         <v>1001.1666666666666</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>50</v>
       </c>
@@ -980,7 +993,7 @@
         <v>500.3</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>50</v>
       </c>
@@ -994,7 +1007,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>50</v>
       </c>
@@ -1008,7 +1021,7 @@
         <v>500.3</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f>AVERAGE(A8:A10)</f>
         <v>50</v>
@@ -1026,7 +1039,7 @@
         <v>500.2</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20</v>
       </c>
@@ -1040,7 +1053,7 @@
         <v>299.10000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>20</v>
       </c>
@@ -1054,7 +1067,7 @@
         <v>299.7</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20</v>
       </c>
@@ -1068,7 +1081,7 @@
         <v>300.39999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f>AVERAGE(A13:A15)</f>
         <v>20</v>
@@ -1086,7 +1099,7 @@
         <v>299.73333333333329</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10</v>
       </c>
@@ -1100,7 +1113,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10</v>
       </c>
@@ -1114,7 +1127,7 @@
         <v>202.6</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10</v>
       </c>
@@ -1128,7 +1141,7 @@
         <v>200.5</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f>AVERAGE(A18:A20)</f>
         <v>10</v>
@@ -1146,7 +1159,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>310</v>
       </c>
@@ -1160,7 +1173,7 @@
         <v>98.5</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>310</v>
       </c>
@@ -1174,7 +1187,7 @@
         <v>101.1</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>310</v>
       </c>
@@ -1188,7 +1201,7 @@
         <v>99.1</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f>AVERAGE(A23:A25)</f>
         <v>310</v>
@@ -1206,7 +1219,7 @@
         <v>99.566666666666663</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1214,7 +1227,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1228,7 +1241,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>10</v>
       </c>
@@ -1244,7 +1257,7 @@
         <v>99.945020000000042</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>20</v>
       </c>
@@ -1260,7 +1273,7 @@
         <v>201.7638</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>50</v>
       </c>
@@ -1276,7 +1289,7 @@
         <v>300.87231999999966</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>205</v>
       </c>
@@ -1292,7 +1305,7 @@
         <v>502.10075999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>310</v>
       </c>
@@ -1318,4 +1331,560 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>0.97340000000000004</v>
+      </c>
+      <c r="C1">
+        <f>(1/B1)</f>
+        <v>1.0273268954181221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <f>1.027327*A4</f>
+        <v>10.27327</v>
+      </c>
+      <c r="C4">
+        <f>(57/1)*(A4/1000)</f>
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="D4" s="2">
+        <f>(57/1)*(B4/1000)</f>
+        <v>0.58557638999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ref="B5:B11" si="0">1.027327*A5</f>
+        <v>20.54654</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:D11" si="1">(57/1)*(A5/1000)</f>
+        <v>1.1400000000000001</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1711527799999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>30.819810000000004</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>1.71</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="1"/>
+        <v>1.7567291700000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>40</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>41.09308</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>2.2800000000000002</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="1"/>
+        <v>2.3423055599999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>51.366350000000004</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>2.85</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="1"/>
+        <v>2.9278819500000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>100</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>102.73270000000001</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>5.7</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="1"/>
+        <v>5.8557639000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>200</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>205.46540000000002</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>11.4</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="1"/>
+        <v>11.711527800000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>300</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>308.19810000000001</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>17.099999999999998</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="1"/>
+        <v>17.567291700000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <f>(57/100)*A18</f>
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <f t="shared" ref="B19:B57" si="2">(57/100)*A19</f>
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="2"/>
+        <v>1.71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="2"/>
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="2"/>
+        <v>2.8499999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="2"/>
+        <v>3.42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="2"/>
+        <v>3.9899999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="2"/>
+        <v>4.5599999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="2"/>
+        <v>5.13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="2"/>
+        <v>5.6999999999999993</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>11</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="2"/>
+        <v>6.27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>12</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="2"/>
+        <v>6.84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>13</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="2"/>
+        <v>7.4099999999999993</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>14</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="2"/>
+        <v>7.9799999999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>15</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="2"/>
+        <v>8.5499999999999989</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>16</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="2"/>
+        <v>9.1199999999999992</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>17</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="2"/>
+        <v>9.69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>18</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="2"/>
+        <v>10.26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>19</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="2"/>
+        <v>10.829999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>20</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="2"/>
+        <v>11.399999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>21</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="2"/>
+        <v>11.969999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>22</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="2"/>
+        <v>12.54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>23</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="2"/>
+        <v>13.11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>24</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="2"/>
+        <v>13.68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>25</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="2"/>
+        <v>14.249999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>26</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="2"/>
+        <v>14.819999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>27</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="2"/>
+        <v>15.389999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>28</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="2"/>
+        <v>15.959999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>29</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="2"/>
+        <v>16.529999999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>30</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="2"/>
+        <v>17.099999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>31</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="2"/>
+        <v>17.669999999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>32</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="2"/>
+        <v>18.239999999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>33</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="2"/>
+        <v>18.809999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>34</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="2"/>
+        <v>19.38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>35</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="2"/>
+        <v>19.95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>36</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="2"/>
+        <v>20.52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>37</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="2"/>
+        <v>21.09</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>38</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="2"/>
+        <v>21.659999999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>39</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="2"/>
+        <v>22.229999999999997</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>40</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="2"/>
+        <v>22.799999999999997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>